<commit_message>
Yazilim araclari: jenkins ve sonar kurulum ayar, not guncelleme
</commit_message>
<xml_diff>
--- a/SoftwareDevEnvAndTools_2017Autumn/_docs/SoftDevEnvandToolsAutumun2017.xlsx
+++ b/SoftwareDevEnvAndTools_2017Autumn/_docs/SoftDevEnvandToolsAutumun2017.xlsx
@@ -1358,7 +1358,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1587,7 +1587,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="8">
-        <f t="shared" ref="K3:K34" si="2">100*SUM(D4:J4)/(2*A$1)</f>
+        <f t="shared" ref="K4:K34" si="2">100*SUM(D4:J4)/(2*A$1)</f>
         <v>100</v>
       </c>
       <c r="L4" s="12">
@@ -2314,11 +2314,13 @@
         <f t="shared" si="0"/>
         <v>68.333333333333329</v>
       </c>
-      <c r="T14" s="8"/>
+      <c r="T14" s="8">
+        <v>50</v>
+      </c>
       <c r="U14" s="12"/>
       <c r="V14" s="17">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
yazilim araclari vize notlar
</commit_message>
<xml_diff>
--- a/SoftwareDevEnvAndTools_2017Autumn/_docs/SoftDevEnvandToolsAutumun2017.xlsx
+++ b/SoftwareDevEnvAndTools_2017Autumn/_docs/SoftDevEnvandToolsAutumun2017.xlsx
@@ -1358,7 +1358,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomLeft" activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1487,16 +1487,16 @@
     </row>
     <row r="3" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="D3" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="18">
         <v>2</v>
@@ -1508,7 +1508,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="18">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="I3" s="18">
         <v>2</v>
@@ -1518,19 +1518,19 @@
       </c>
       <c r="K3" s="8">
         <f>100*SUM(D3:J3)/(2*A$1)</f>
-        <v>115.83333333333333</v>
+        <v>100</v>
       </c>
       <c r="L3" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M3" s="11">
         <v>100</v>
       </c>
       <c r="N3" s="11">
+        <v>90</v>
+      </c>
+      <c r="O3" s="11">
         <v>80</v>
-      </c>
-      <c r="O3" s="11">
-        <v>70</v>
       </c>
       <c r="P3" s="11">
         <v>85</v>
@@ -1543,30 +1543,32 @@
         <v>90</v>
       </c>
       <c r="S3" s="8">
-        <f t="shared" ref="S3:S34" si="0">SUM(L3:R3)/(A$1)</f>
-        <v>104.16666666666667</v>
+        <f>SUM(L3:R3)/(A$1)</f>
+        <v>90.833333333333329</v>
       </c>
       <c r="T3" s="8">
-        <v>75</v>
-      </c>
-      <c r="U3" s="12"/>
+        <v>100</v>
+      </c>
+      <c r="U3" s="8">
+        <v>100</v>
+      </c>
       <c r="V3" s="17">
-        <f t="shared" ref="V3:V34" si="1">K3*0.2+S3*0.2+T3*0.25+U3*0.35</f>
-        <v>62.75</v>
+        <f>K3*0.2+S3*0.2+T3*0.25+U3*0.35+2</f>
+        <v>100.16666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="D4" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" s="18">
         <v>2</v>
@@ -1578,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="18">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="I4" s="18">
         <v>2</v>
@@ -1587,20 +1589,20 @@
         <v>2</v>
       </c>
       <c r="K4" s="8">
-        <f t="shared" ref="K4:K34" si="2">100*SUM(D4:J4)/(2*A$1)</f>
+        <f>100*SUM(D4:J4)/(2*A$1)</f>
+        <v>115.83333333333333</v>
+      </c>
+      <c r="L4" s="12">
         <v>100</v>
-      </c>
-      <c r="L4" s="12">
-        <v>0</v>
       </c>
       <c r="M4" s="11">
         <v>100</v>
       </c>
       <c r="N4" s="11">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="O4" s="11">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="P4" s="11">
         <v>85</v>
@@ -1609,20 +1611,22 @@
         <v>100</v>
       </c>
       <c r="R4" s="11">
-        <f t="shared" ref="R4:R13" si="3">J4*50-10</f>
+        <f>J4*50-10</f>
         <v>90</v>
       </c>
       <c r="S4" s="8">
-        <f t="shared" si="0"/>
-        <v>90.833333333333329</v>
+        <f>SUM(L4:R4)/(A$1)</f>
+        <v>104.16666666666667</v>
       </c>
       <c r="T4" s="8">
-        <v>100</v>
-      </c>
-      <c r="U4" s="12"/>
+        <v>75</v>
+      </c>
+      <c r="U4" s="8">
+        <v>72</v>
+      </c>
       <c r="V4" s="17">
-        <f t="shared" si="1"/>
-        <v>63.166666666666671</v>
+        <f t="shared" ref="V4:V34" si="0">K4*0.2+S4*0.2+T4*0.25+U4*0.35+2</f>
+        <v>89.95</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1657,7 +1661,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D5:J5)/(2*A$1)</f>
         <v>100</v>
       </c>
       <c r="L5" s="12">
@@ -1679,38 +1683,42 @@
         <v>100</v>
       </c>
       <c r="R5" s="11">
-        <f t="shared" si="3"/>
+        <f>J5*50-10</f>
         <v>90</v>
       </c>
       <c r="S5" s="8">
-        <f t="shared" si="0"/>
+        <f>SUM(L5:R5)/(A$1)</f>
         <v>89.166666666666671</v>
       </c>
       <c r="T5" s="8">
         <v>75</v>
       </c>
-      <c r="U5" s="12"/>
+      <c r="U5" s="8">
+        <v>82</v>
+      </c>
       <c r="V5" s="17">
-        <f t="shared" si="1"/>
-        <v>56.583333333333336</v>
+        <f t="shared" si="0"/>
+        <v>87.283333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="19"/>
+        <v>113</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0</v>
+      </c>
       <c r="E6" s="18">
         <v>2</v>
       </c>
       <c r="F6" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" s="18">
         <v>2</v>
@@ -1725,8 +1733,8 @@
         <v>2</v>
       </c>
       <c r="K6" s="8">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f>100*SUM(D6:J6)/(2*A$1)</f>
+        <v>83.333333333333329</v>
       </c>
       <c r="L6" s="12">
         <v>0</v>
@@ -1735,7 +1743,7 @@
         <v>100</v>
       </c>
       <c r="N6" s="11">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="O6" s="11">
         <v>80</v>
@@ -1747,40 +1755,40 @@
         <v>100</v>
       </c>
       <c r="R6" s="11">
-        <f t="shared" si="3"/>
+        <f>J6*50-10</f>
         <v>90</v>
       </c>
       <c r="S6" s="8">
+        <f>SUM(L6:R6)/(A$1)</f>
+        <v>75.833333333333329</v>
+      </c>
+      <c r="T6" s="8">
+        <v>100</v>
+      </c>
+      <c r="U6" s="8">
+        <v>80</v>
+      </c>
+      <c r="V6" s="17">
         <f t="shared" si="0"/>
-        <v>89.166666666666671</v>
-      </c>
-      <c r="T6" s="8">
-        <v>75</v>
-      </c>
-      <c r="U6" s="12"/>
-      <c r="V6" s="17">
-        <f t="shared" si="1"/>
-        <v>56.583333333333336</v>
+        <v>86.833333333333343</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D7" s="19"/>
       <c r="E7" s="18">
         <v>2</v>
       </c>
       <c r="F7" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" s="18">
         <v>2</v>
@@ -1795,8 +1803,8 @@
         <v>2</v>
       </c>
       <c r="K7" s="8">
-        <f t="shared" si="2"/>
-        <v>83.333333333333329</v>
+        <f>100*SUM(D7:J7)/(2*A$1)</f>
+        <v>100</v>
       </c>
       <c r="L7" s="12">
         <v>0</v>
@@ -1805,7 +1813,7 @@
         <v>100</v>
       </c>
       <c r="N7" s="11">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="O7" s="11">
         <v>80</v>
@@ -1817,20 +1825,22 @@
         <v>100</v>
       </c>
       <c r="R7" s="11">
-        <f t="shared" si="3"/>
+        <f>J7*50-10</f>
         <v>90</v>
       </c>
       <c r="S7" s="8">
+        <f>SUM(L7:R7)/(A$1)</f>
+        <v>89.166666666666671</v>
+      </c>
+      <c r="T7" s="8">
+        <v>75</v>
+      </c>
+      <c r="U7" s="8">
+        <v>75</v>
+      </c>
+      <c r="V7" s="17">
         <f t="shared" si="0"/>
-        <v>75.833333333333329</v>
-      </c>
-      <c r="T7" s="8">
-        <v>100</v>
-      </c>
-      <c r="U7" s="12"/>
-      <c r="V7" s="17">
-        <f t="shared" si="1"/>
-        <v>56.833333333333336</v>
+        <v>84.833333333333343</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1865,7 +1875,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D8:J8)/(2*A$1)</f>
         <v>75</v>
       </c>
       <c r="L8" s="12">
@@ -1887,20 +1897,22 @@
         <v>100</v>
       </c>
       <c r="R8" s="11">
-        <f t="shared" si="3"/>
+        <f>J8*50-10</f>
         <v>90</v>
       </c>
       <c r="S8" s="8">
-        <f t="shared" si="0"/>
+        <f>SUM(L8:R8)/(A$1)</f>
         <v>77.5</v>
       </c>
       <c r="T8" s="8">
         <v>95</v>
       </c>
-      <c r="U8" s="12"/>
+      <c r="U8" s="8">
+        <v>61</v>
+      </c>
       <c r="V8" s="17">
-        <f t="shared" si="1"/>
-        <v>54.25</v>
+        <f t="shared" si="0"/>
+        <v>77.599999999999994</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1935,7 +1947,7 @@
         <v>2</v>
       </c>
       <c r="K9" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D9:J9)/(2*A$1)</f>
         <v>80.833333333333329</v>
       </c>
       <c r="L9" s="12">
@@ -1957,20 +1969,22 @@
         <v>100</v>
       </c>
       <c r="R9" s="11">
-        <f t="shared" si="3"/>
+        <f>J9*50-10</f>
         <v>90</v>
       </c>
       <c r="S9" s="8">
-        <f t="shared" si="0"/>
+        <f>SUM(L9:R9)/(A$1)</f>
         <v>74.166666666666671</v>
       </c>
       <c r="T9" s="8">
         <v>90</v>
       </c>
-      <c r="U9" s="12"/>
+      <c r="U9" s="8">
+        <v>54</v>
+      </c>
       <c r="V9" s="17">
-        <f t="shared" si="1"/>
-        <v>53.5</v>
+        <f t="shared" si="0"/>
+        <v>74.400000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2005,7 +2019,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D10:J10)/(2*A$1)</f>
         <v>75</v>
       </c>
       <c r="L10" s="12">
@@ -2027,43 +2041,45 @@
         <v>100</v>
       </c>
       <c r="R10" s="11">
-        <f t="shared" si="3"/>
+        <f>J10*50-10</f>
         <v>90</v>
       </c>
       <c r="S10" s="8">
-        <f t="shared" si="0"/>
+        <f>SUM(L10:R10)/(A$1)</f>
         <v>75</v>
       </c>
       <c r="T10" s="8">
         <v>80</v>
       </c>
-      <c r="U10" s="12"/>
+      <c r="U10" s="8">
+        <v>53</v>
+      </c>
       <c r="V10" s="17">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>70.55</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="D11" s="19">
         <v>0</v>
       </c>
       <c r="E11" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11" s="18">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H11" s="18">
         <v>2</v>
@@ -2075,20 +2091,20 @@
         <v>2</v>
       </c>
       <c r="K11" s="8">
-        <f t="shared" si="2"/>
-        <v>79.166666666666671</v>
+        <f>100*SUM(D11:J11)/(2*A$1)</f>
+        <v>66.666666666666671</v>
       </c>
       <c r="L11" s="12">
         <v>0</v>
       </c>
       <c r="M11" s="11">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N11" s="11">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="O11" s="11">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="P11" s="12">
         <v>85</v>
@@ -2097,43 +2113,45 @@
         <v>100</v>
       </c>
       <c r="R11" s="11">
-        <f>J11*50-20</f>
-        <v>80</v>
+        <f>J11*50-10</f>
+        <v>90</v>
       </c>
       <c r="S11" s="8">
+        <f>SUM(L11:R11)/(A$1)</f>
+        <v>59.166666666666664</v>
+      </c>
+      <c r="T11" s="8">
+        <v>75</v>
+      </c>
+      <c r="U11" s="8">
+        <v>69</v>
+      </c>
+      <c r="V11" s="17">
         <f t="shared" si="0"/>
-        <v>67.5</v>
-      </c>
-      <c r="T11" s="8">
-        <v>70</v>
-      </c>
-      <c r="U11" s="12"/>
-      <c r="V11" s="17">
-        <f t="shared" si="1"/>
-        <v>46.833333333333336</v>
+        <v>70.066666666666663</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="D12" s="19">
         <v>0</v>
       </c>
       <c r="E12" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" s="18">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H12" s="18">
         <v>2</v>
@@ -2145,20 +2163,20 @@
         <v>2</v>
       </c>
       <c r="K12" s="8">
-        <f t="shared" si="2"/>
-        <v>66.666666666666671</v>
+        <f>100*SUM(D12:J12)/(2*A$1)</f>
+        <v>79.166666666666671</v>
       </c>
       <c r="L12" s="12">
         <v>0</v>
       </c>
       <c r="M12" s="11">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="N12" s="11">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="O12" s="11">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="P12" s="11">
         <v>85</v>
@@ -2167,160 +2185,166 @@
         <v>100</v>
       </c>
       <c r="R12" s="11">
-        <f t="shared" si="3"/>
-        <v>90</v>
+        <f>J12*50-20</f>
+        <v>80</v>
       </c>
       <c r="S12" s="8">
+        <f>SUM(L12:R12)/(A$1)</f>
+        <v>67.5</v>
+      </c>
+      <c r="T12" s="8">
+        <v>70</v>
+      </c>
+      <c r="U12" s="8">
+        <v>60</v>
+      </c>
+      <c r="V12" s="17">
         <f t="shared" si="0"/>
-        <v>59.166666666666664</v>
-      </c>
-      <c r="T12" s="8">
-        <v>75</v>
-      </c>
-      <c r="U12" s="12"/>
-      <c r="V12" s="17">
-        <f t="shared" si="1"/>
-        <v>43.916666666666671</v>
+        <v>69.833333333333343</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="D13" s="19">
         <v>0</v>
       </c>
       <c r="E13" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" s="18">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="I13" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13" s="18">
         <v>2</v>
       </c>
       <c r="K13" s="8">
-        <f t="shared" si="2"/>
-        <v>63.333333333333336</v>
+        <f>100*SUM(D13:J13)/(2*A$1)</f>
+        <v>66.666666666666671</v>
       </c>
       <c r="L13" s="12">
         <v>0</v>
       </c>
       <c r="M13" s="11">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N13" s="11">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="O13" s="11">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P13" s="12">
         <v>90</v>
       </c>
       <c r="Q13" s="11">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="R13" s="11">
-        <f t="shared" si="3"/>
-        <v>90</v>
+        <f>J13*50-20</f>
+        <v>80</v>
       </c>
       <c r="S13" s="8">
+        <f>SUM(L13:R13)/(A$1)</f>
+        <v>68.333333333333329</v>
+      </c>
+      <c r="T13" s="8">
+        <v>50</v>
+      </c>
+      <c r="U13" s="8">
+        <v>54</v>
+      </c>
+      <c r="V13" s="17">
         <f t="shared" si="0"/>
-        <v>61.666666666666664</v>
-      </c>
-      <c r="T13" s="8">
-        <v>60</v>
-      </c>
-      <c r="U13" s="12"/>
-      <c r="V13" s="17">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <v>60.4</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="D14" s="19">
         <v>0</v>
       </c>
       <c r="E14" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H14" s="18">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="I14" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="18">
         <v>2</v>
       </c>
       <c r="K14" s="8">
-        <f t="shared" si="2"/>
-        <v>66.666666666666671</v>
+        <f>100*SUM(D14:J14)/(2*A$1)</f>
+        <v>63.333333333333336</v>
       </c>
       <c r="L14" s="12">
         <v>0</v>
       </c>
       <c r="M14" s="11">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="N14" s="11">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O14" s="11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="P14" s="12">
         <v>90</v>
       </c>
       <c r="Q14" s="11">
+        <v>100</v>
+      </c>
+      <c r="R14" s="11">
+        <f>J14*50-10</f>
+        <v>90</v>
+      </c>
+      <c r="S14" s="8">
+        <f>SUM(L14:R14)/(A$1)</f>
+        <v>61.666666666666664</v>
+      </c>
+      <c r="T14" s="8">
         <v>60</v>
       </c>
-      <c r="R14" s="11">
-        <f>J14*50-20</f>
-        <v>80</v>
-      </c>
-      <c r="S14" s="8">
+      <c r="U14" s="8">
+        <v>50</v>
+      </c>
+      <c r="V14" s="17">
         <f t="shared" si="0"/>
-        <v>68.333333333333329</v>
-      </c>
-      <c r="T14" s="8">
-        <v>50</v>
-      </c>
-      <c r="U14" s="12"/>
-      <c r="V14" s="17">
-        <f t="shared" si="1"/>
-        <v>39.5</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2355,7 +2379,7 @@
         <v>2</v>
       </c>
       <c r="K15" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D15:J15)/(2*A$1)</f>
         <v>41.666666666666664</v>
       </c>
       <c r="L15" s="12">
@@ -2381,14 +2405,16 @@
         <v>80</v>
       </c>
       <c r="S15" s="8">
+        <f>SUM(L15:R15)/(A$1)</f>
+        <v>43.333333333333336</v>
+      </c>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8">
+        <v>26</v>
+      </c>
+      <c r="V15" s="17">
         <f t="shared" si="0"/>
-        <v>43.333333333333336</v>
-      </c>
-      <c r="T15" s="8"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="17">
-        <f t="shared" si="1"/>
-        <v>17</v>
+        <v>28.1</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2423,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D16:J16)/(2*A$1)</f>
         <v>35.833333333333336</v>
       </c>
       <c r="L16" s="12">
@@ -2445,18 +2471,20 @@
         <v>30</v>
       </c>
       <c r="R16" s="11">
-        <f t="shared" ref="R16:R34" si="4">J16*50</f>
+        <f>J16*50</f>
         <v>0</v>
       </c>
       <c r="S16" s="8">
+        <f>SUM(L16:R16)/(A$1)</f>
+        <v>27.5</v>
+      </c>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8">
+        <v>22</v>
+      </c>
+      <c r="V16" s="17">
         <f t="shared" si="0"/>
-        <v>27.5</v>
-      </c>
-      <c r="T16" s="8"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="17">
-        <f t="shared" si="1"/>
-        <v>12.666666666666668</v>
+        <v>22.366666666666667</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2491,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D17:J17)/(2*A$1)</f>
         <v>25</v>
       </c>
       <c r="L17" s="12">
@@ -2513,234 +2541,240 @@
         <v>100</v>
       </c>
       <c r="R17" s="11">
-        <f t="shared" si="4"/>
+        <f>J17*50</f>
         <v>0</v>
       </c>
       <c r="S17" s="8">
+        <f>SUM(L17:R17)/(A$1)</f>
+        <v>30</v>
+      </c>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8">
+        <v>22</v>
+      </c>
+      <c r="V17" s="17">
         <f t="shared" si="0"/>
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="19">
+        <v>0</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="18">
+        <v>2</v>
+      </c>
+      <c r="I18" s="18">
+        <v>0</v>
+      </c>
+      <c r="J18" s="18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="8">
+        <f>100*SUM(D18:J18)/(2*A$1)</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L18" s="12">
+        <v>0</v>
+      </c>
+      <c r="M18" s="11">
+        <v>0</v>
+      </c>
+      <c r="N18" s="11">
+        <v>0</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0</v>
+      </c>
+      <c r="P18" s="11">
+        <v>85</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
+        <f>J18*50</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="8">
+        <f>SUM(L18:R18)/(A$1)</f>
+        <v>14.166666666666666</v>
+      </c>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8">
         <v>30</v>
       </c>
-      <c r="T17" s="8"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="17">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="D18" s="19">
-        <v>0</v>
-      </c>
-      <c r="E18" s="18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="18">
-        <v>0</v>
-      </c>
-      <c r="H18" s="18">
-        <v>0</v>
-      </c>
-      <c r="I18" s="18">
-        <v>2</v>
-      </c>
-      <c r="J18" s="18">
-        <v>0</v>
-      </c>
-      <c r="K18" s="8">
-        <f t="shared" si="2"/>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="L18" s="12">
-        <v>0</v>
-      </c>
-      <c r="M18" s="11">
-        <v>0</v>
-      </c>
-      <c r="N18" s="11">
-        <v>0</v>
-      </c>
-      <c r="O18" s="11">
-        <v>0</v>
-      </c>
-      <c r="P18" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="11">
-        <v>100</v>
-      </c>
-      <c r="R18" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S18" s="8">
+      <c r="V18" s="17">
         <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="T18" s="8"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="17">
-        <f t="shared" si="1"/>
-        <v>6.6666666666666679</v>
+        <v>18.666666666666668</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="18">
+        <v>0</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0</v>
+      </c>
+      <c r="F19" s="18">
+        <v>0</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0</v>
+      </c>
+      <c r="H19" s="18">
+        <v>0</v>
+      </c>
+      <c r="I19" s="18">
+        <v>0</v>
+      </c>
+      <c r="J19" s="18">
+        <v>0</v>
+      </c>
+      <c r="K19" s="8">
+        <f>100*SUM(D19:J19)/(2*A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
+        <v>0</v>
+      </c>
+      <c r="M19" s="12">
+        <v>0</v>
+      </c>
+      <c r="N19" s="12">
+        <v>0</v>
+      </c>
+      <c r="O19" s="12">
+        <v>0</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>0</v>
+      </c>
+      <c r="R19" s="11">
+        <f>J19*50</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="8">
+        <f>SUM(L19:R19)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8">
+        <v>26</v>
+      </c>
+      <c r="V19" s="17">
+        <f t="shared" si="0"/>
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="18">
+        <v>0</v>
+      </c>
+      <c r="E20" s="18">
+        <v>0</v>
+      </c>
+      <c r="F20" s="18">
+        <v>0</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0</v>
+      </c>
+      <c r="H20" s="18">
+        <v>0</v>
+      </c>
+      <c r="I20" s="18">
+        <v>2</v>
+      </c>
+      <c r="J20" s="18">
+        <v>0</v>
+      </c>
+      <c r="K20" s="8">
+        <f>100*SUM(D20:J20)/(2*A$1)</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L20" s="12">
+        <v>0</v>
+      </c>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20" s="12">
+        <v>0</v>
+      </c>
+      <c r="O20" s="12">
+        <v>0</v>
+      </c>
+      <c r="P20" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="11">
         <v>100</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="18">
-        <v>0</v>
-      </c>
-      <c r="E19" s="18">
-        <v>0</v>
-      </c>
-      <c r="F19" s="18">
-        <v>0</v>
-      </c>
-      <c r="G19" s="18">
-        <v>0</v>
-      </c>
-      <c r="H19" s="18">
-        <v>2</v>
-      </c>
-      <c r="I19" s="18">
-        <v>0</v>
-      </c>
-      <c r="J19" s="18">
-        <v>0</v>
-      </c>
-      <c r="K19" s="8">
-        <f t="shared" si="2"/>
+      <c r="R20" s="11">
+        <f>J20*50</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="8">
+        <f>SUM(L20:R20)/(A$1)</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="L19" s="12">
-        <v>0</v>
-      </c>
-      <c r="M19" s="12">
-        <v>0</v>
-      </c>
-      <c r="N19" s="12">
-        <v>0</v>
-      </c>
-      <c r="O19" s="12">
-        <v>0</v>
-      </c>
-      <c r="P19" s="12">
-        <v>85</v>
-      </c>
-      <c r="Q19" s="11">
-        <v>0</v>
-      </c>
-      <c r="R19" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S19" s="8">
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="17">
         <f t="shared" si="0"/>
-        <v>14.166666666666666</v>
-      </c>
-      <c r="T19" s="8"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="17">
-        <f t="shared" si="1"/>
-        <v>6.1666666666666679</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="18">
-        <v>0</v>
-      </c>
-      <c r="E20" s="18">
-        <v>1.25</v>
-      </c>
-      <c r="F20" s="18">
-        <v>0</v>
-      </c>
-      <c r="G20" s="18">
-        <v>0</v>
-      </c>
-      <c r="H20" s="18">
-        <v>0</v>
-      </c>
-      <c r="I20" s="18">
-        <v>0</v>
-      </c>
-      <c r="J20" s="18">
-        <v>0</v>
-      </c>
-      <c r="K20" s="8">
-        <f t="shared" si="2"/>
-        <v>10.416666666666666</v>
-      </c>
-      <c r="L20" s="12">
-        <v>0</v>
-      </c>
-      <c r="M20" s="12">
-        <v>85</v>
-      </c>
-      <c r="N20" s="12">
-        <v>0</v>
-      </c>
-      <c r="O20" s="12">
-        <v>0</v>
-      </c>
-      <c r="P20" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="11">
-        <v>0</v>
-      </c>
-      <c r="R20" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S20" s="8">
-        <f t="shared" si="0"/>
-        <v>14.166666666666666</v>
-      </c>
-      <c r="T20" s="8"/>
-      <c r="U20" s="12"/>
-      <c r="V20" s="17">
-        <f t="shared" si="1"/>
-        <v>4.916666666666667</v>
+        <v>8.6666666666666679</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D21" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="18">
         <v>0</v>
@@ -2761,11 +2795,11 @@
         <v>0</v>
       </c>
       <c r="K21" s="8">
-        <f t="shared" si="2"/>
-        <v>8.3333333333333339</v>
+        <f>100*SUM(D21:J21)/(2*A$1)</f>
+        <v>0</v>
       </c>
       <c r="L21" s="12">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M21" s="12">
         <v>0</v>
@@ -2783,32 +2817,31 @@
         <v>0</v>
       </c>
       <c r="R21" s="11">
-        <f t="shared" si="4"/>
+        <f>J21*50</f>
         <v>0</v>
       </c>
       <c r="S21" s="8">
+        <f>SUM(L21:R21)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8">
+        <v>19</v>
+      </c>
+      <c r="V21" s="17">
         <f t="shared" si="0"/>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="T21" s="8"/>
-      <c r="U21" s="12"/>
-      <c r="V21" s="17">
-        <f t="shared" si="1"/>
-        <v>4.3333333333333339</v>
-      </c>
-      <c r="W21" s="2" t="s">
-        <v>62</v>
+        <v>8.6499999999999986</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="D22" s="18">
         <v>0</v>
@@ -2832,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D22:J22)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L22" s="12">
@@ -2854,35 +2887,37 @@
         <v>0</v>
       </c>
       <c r="R22" s="11">
-        <f t="shared" si="4"/>
+        <f>J22*50</f>
         <v>0</v>
       </c>
       <c r="S22" s="8">
+        <f>SUM(L22:R22)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8">
+        <v>18</v>
+      </c>
+      <c r="V22" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T22" s="8"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D23" s="18">
         <v>0</v>
       </c>
       <c r="E23" s="18">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="F23" s="18">
         <v>0</v>
@@ -2900,14 +2935,14 @@
         <v>0</v>
       </c>
       <c r="K23" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>100*SUM(D23:J23)/(2*A$1)</f>
+        <v>10.416666666666666</v>
       </c>
       <c r="L23" s="12">
         <v>0</v>
       </c>
       <c r="M23" s="11">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="N23" s="12">
         <v>0</v>
@@ -2922,32 +2957,32 @@
         <v>0</v>
       </c>
       <c r="R23" s="11">
-        <f t="shared" si="4"/>
+        <f>J23*50</f>
         <v>0</v>
       </c>
       <c r="S23" s="8">
+        <f>SUM(L23:R23)/(A$1)</f>
+        <v>14.166666666666666</v>
+      </c>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T23" s="8"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.916666666666667</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D24" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="18">
         <v>0</v>
@@ -2968,11 +3003,11 @@
         <v>0</v>
       </c>
       <c r="K24" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>100*SUM(D24:J24)/(2*A$1)</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="L24" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M24" s="12">
         <v>0</v>
@@ -2990,29 +3025,32 @@
         <v>0</v>
       </c>
       <c r="R24" s="11">
-        <f t="shared" si="4"/>
+        <f>J24*50</f>
         <v>0</v>
       </c>
       <c r="S24" s="8">
+        <f>SUM(L24:R24)/(A$1)</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T24" s="8"/>
-      <c r="U24" s="12"/>
-      <c r="V24" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.3333333333333339</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D25" s="18">
         <v>0</v>
@@ -3036,7 +3074,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D25:J25)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L25" s="12">
@@ -3058,29 +3096,29 @@
         <v>0</v>
       </c>
       <c r="R25" s="11">
-        <f t="shared" si="4"/>
+        <f>J25*50</f>
         <v>0</v>
       </c>
       <c r="S25" s="8">
+        <f>SUM(L25:R25)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T25" s="8"/>
-      <c r="U25" s="12"/>
-      <c r="V25" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D26" s="18">
         <v>0</v>
@@ -3104,7 +3142,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D26:J26)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L26" s="12">
@@ -3126,29 +3164,29 @@
         <v>0</v>
       </c>
       <c r="R26" s="11">
-        <f t="shared" si="4"/>
+        <f>J26*50</f>
         <v>0</v>
       </c>
       <c r="S26" s="8">
+        <f>SUM(L26:R26)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T26" s="8"/>
-      <c r="U26" s="12"/>
-      <c r="V26" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D27" s="18">
         <v>0</v>
@@ -3172,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D27:J27)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L27" s="12">
@@ -3194,29 +3232,29 @@
         <v>0</v>
       </c>
       <c r="R27" s="11">
-        <f t="shared" si="4"/>
+        <f>J27*50</f>
         <v>0</v>
       </c>
       <c r="S27" s="8">
+        <f>SUM(L27:R27)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T27" s="8"/>
-      <c r="U27" s="12"/>
-      <c r="V27" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D28" s="18">
         <v>0</v>
@@ -3240,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D28:J28)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L28" s="12">
@@ -3262,29 +3300,29 @@
         <v>0</v>
       </c>
       <c r="R28" s="11">
-        <f t="shared" si="4"/>
+        <f>J28*50</f>
         <v>0</v>
       </c>
       <c r="S28" s="8">
+        <f>SUM(L28:R28)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T28" s="8"/>
-      <c r="U28" s="12"/>
-      <c r="V28" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>108</v>
+        <v>36</v>
       </c>
       <c r="D29" s="18">
         <v>0</v>
@@ -3308,7 +3346,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D29:J29)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L29" s="12">
@@ -3330,29 +3368,29 @@
         <v>0</v>
       </c>
       <c r="R29" s="11">
-        <f t="shared" si="4"/>
+        <f>J29*50</f>
         <v>0</v>
       </c>
       <c r="S29" s="8">
+        <f>SUM(L29:R29)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T29" s="8"/>
-      <c r="U29" s="12"/>
-      <c r="V29" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D30" s="18">
         <v>0</v>
@@ -3376,7 +3414,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D30:J30)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L30" s="12">
@@ -3398,29 +3436,29 @@
         <v>0</v>
       </c>
       <c r="R30" s="11">
-        <f t="shared" si="4"/>
+        <f>J30*50</f>
         <v>0</v>
       </c>
       <c r="S30" s="8">
+        <f>SUM(L30:R30)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T30" s="8"/>
-      <c r="U30" s="12"/>
-      <c r="V30" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="D31" s="18">
         <v>0</v>
@@ -3444,7 +3482,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D31:J31)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L31" s="12">
@@ -3466,18 +3504,18 @@
         <v>0</v>
       </c>
       <c r="R31" s="11">
-        <f t="shared" si="4"/>
+        <f>J31*50</f>
         <v>0</v>
       </c>
       <c r="S31" s="8">
+        <f>SUM(L31:R31)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T31" s="8"/>
-      <c r="U31" s="12"/>
-      <c r="V31" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3512,7 +3550,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D32:J32)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L32" s="12">
@@ -3534,18 +3572,18 @@
         <v>0</v>
       </c>
       <c r="R32" s="11">
-        <f t="shared" si="4"/>
+        <f>J32*50</f>
         <v>0</v>
       </c>
       <c r="S32" s="8">
+        <f>SUM(L32:R32)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T32" s="8"/>
-      <c r="U32" s="12"/>
-      <c r="V32" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3580,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D33:J33)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L33" s="12">
@@ -3602,18 +3640,18 @@
         <v>0</v>
       </c>
       <c r="R33" s="11">
-        <f t="shared" si="4"/>
+        <f>J33*50</f>
         <v>0</v>
       </c>
       <c r="S33" s="8">
+        <f>SUM(L33:R33)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T33" s="8"/>
-      <c r="U33" s="12"/>
-      <c r="V33" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3648,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="8">
-        <f t="shared" si="2"/>
+        <f>100*SUM(D34:J34)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L34" s="12">
@@ -3670,18 +3708,18 @@
         <v>0</v>
       </c>
       <c r="R34" s="11">
-        <f t="shared" si="4"/>
+        <f>J34*50</f>
         <v>0</v>
       </c>
       <c r="S34" s="8">
+        <f>SUM(L34:R34)/(A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T34" s="10"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T34" s="10"/>
-      <c r="U34" s="7"/>
-      <c r="V34" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:22" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4736,19 +4774,19 @@
     <mergeCell ref="L1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:J34">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K34">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4762,7 +4800,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S34">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4776,7 +4814,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T34">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4790,7 +4828,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V34">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4804,20 +4842,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:R34">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
       <formula>80</formula>
       <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3:U34">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8714777B-A242-4EFE-98F1-D51B58F1BB53}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4869,6 +4921,17 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>V3:V34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8714777B-A242-4EFE-98F1-D51B58F1BB53}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U3:U34</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
yazilim araclari 2. hafta sonrasi notlar
</commit_message>
<xml_diff>
--- a/SoftwareDevEnvAndTools_2017Autumn/_docs/SoftDevEnvandToolsAutumun2017.xlsx
+++ b/SoftwareDevEnvAndTools_2017Autumn/_docs/SoftDevEnvandToolsAutumun2017.xlsx
@@ -973,7 +973,45 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1650,7 +1688,7 @@
         <v>100</v>
       </c>
       <c r="V3" s="17">
-        <f t="shared" ref="V3:V34" si="3">K3*0.2+S3*0.2+T3*0.25+U3*0.35+2</f>
+        <f t="shared" ref="V3:V24" si="3">K3*0.2+S3*0.2+T3*0.25+U3*0.35+2</f>
         <v>100.16666666666667</v>
       </c>
     </row>
@@ -4861,14 +4899,14 @@
     <mergeCell ref="L1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:J34">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4929,18 +4967,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:R34">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
@@ -5035,7 +5073,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM27" sqref="AM27"/>
+      <selection pane="bottomLeft" activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5067,7 +5105,7 @@
   <sheetData>
     <row r="1" spans="1:35" s="34" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="44"/>
@@ -5243,7 +5281,9 @@
       <c r="E3" s="43">
         <v>2</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="18">
+        <v>2</v>
+      </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
@@ -5256,7 +5296,9 @@
       <c r="M3" s="12">
         <v>80</v>
       </c>
-      <c r="N3" s="11"/>
+      <c r="N3" s="11">
+        <v>100</v>
+      </c>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
@@ -5264,7 +5306,7 @@
       <c r="S3" s="11"/>
       <c r="T3" s="8">
         <f>SUM(M3:S3)/(A$1)</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="U3" s="12"/>
       <c r="V3" s="11"/>
@@ -5287,11 +5329,11 @@
       <c r="AG3" s="12"/>
       <c r="AH3" s="17">
         <f>L3*0.1+T3*0.2+Z3*0.2+AF3*0.2+AG3*0.3</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AI3" s="17">
         <f>D3*0.4+AH3*0.6</f>
-        <v>55.666666666666671</v>
+        <v>56.866666666666674</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5310,7 +5352,9 @@
       <c r="E4" s="43">
         <v>2</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="18">
+        <v>2</v>
+      </c>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
@@ -5323,7 +5367,9 @@
       <c r="M4" s="12">
         <v>80</v>
       </c>
-      <c r="N4" s="11"/>
+      <c r="N4" s="11">
+        <v>100</v>
+      </c>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -5331,7 +5377,7 @@
       <c r="S4" s="11"/>
       <c r="T4" s="8">
         <f>SUM(M4:S4)/(A$1)</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="U4" s="12"/>
       <c r="V4" s="11"/>
@@ -5354,11 +5400,11 @@
       <c r="AG4" s="12"/>
       <c r="AH4" s="17">
         <f>L4*0.1+T4*0.2+Z4*0.2+AF4*0.2+AG4*0.3</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AI4" s="17">
         <f>D4*0.4+AH4*0.6</f>
-        <v>51.580000000000005</v>
+        <v>52.78</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5377,7 +5423,9 @@
       <c r="E5" s="43">
         <v>2</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="18">
+        <v>2</v>
+      </c>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
@@ -5390,7 +5438,9 @@
       <c r="M5" s="12">
         <v>80</v>
       </c>
-      <c r="N5" s="11"/>
+      <c r="N5" s="11">
+        <v>100</v>
+      </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -5398,7 +5448,7 @@
       <c r="S5" s="11"/>
       <c r="T5" s="8">
         <f>SUM(M5:S5)/(A$1)</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="U5" s="12"/>
       <c r="V5" s="11"/>
@@ -5421,30 +5471,32 @@
       <c r="AG5" s="12"/>
       <c r="AH5" s="17">
         <f>L5*0.1+T5*0.2+Z5*0.2+AF5*0.2+AG5*0.3</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AI5" s="17">
         <f>D5*0.4+AH5*0.6</f>
-        <v>50.333333333333343</v>
+        <v>51.533333333333346</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="D6" s="12">
-        <v>77.599999999999994</v>
+        <v>87.283333333333331</v>
       </c>
       <c r="E6" s="43">
-        <v>1.3</v>
-      </c>
-      <c r="F6" s="18"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="18">
+        <v>2</v>
+      </c>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
@@ -5452,12 +5504,14 @@
       <c r="K6" s="18"/>
       <c r="L6" s="8">
         <f>100*SUM(E6:K6)/(2*A$1)</f>
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="M6" s="12">
-        <v>80</v>
-      </c>
-      <c r="N6" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="11">
+        <v>100</v>
+      </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -5465,7 +5519,7 @@
       <c r="S6" s="11"/>
       <c r="T6" s="8">
         <f>SUM(M6:S6)/(A$1)</f>
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="U6" s="12"/>
       <c r="V6" s="11"/>
@@ -5488,30 +5542,32 @@
       <c r="AG6" s="12"/>
       <c r="AH6" s="17">
         <f>L6*0.1+T6*0.2+Z6*0.2+AF6*0.2+AG6*0.3</f>
-        <v>22.5</v>
+        <v>15</v>
       </c>
       <c r="AI6" s="17">
         <f>D6*0.4+AH6*0.6</f>
-        <v>44.54</v>
+        <v>43.913333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="D7" s="12">
-        <v>74.400000000000006</v>
+        <v>84.833333333333343</v>
       </c>
       <c r="E7" s="43">
-        <v>1</v>
-      </c>
-      <c r="F7" s="18"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="18">
+        <v>2</v>
+      </c>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
@@ -5522,9 +5578,11 @@
         <v>50</v>
       </c>
       <c r="M7" s="12">
-        <v>60</v>
-      </c>
-      <c r="N7" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="11">
+        <v>100</v>
+      </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -5532,7 +5590,7 @@
       <c r="S7" s="11"/>
       <c r="T7" s="8">
         <f>SUM(M7:S7)/(A$1)</f>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="U7" s="12"/>
       <c r="V7" s="11"/>
@@ -5555,30 +5613,32 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="17">
         <f>L7*0.1+T7*0.2+Z7*0.2+AF7*0.2+AG7*0.3</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AI7" s="17">
         <f>D7*0.4+AH7*0.6</f>
-        <v>39.960000000000008</v>
+        <v>42.933333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="D8" s="12">
-        <v>60.4</v>
+        <v>70.066666666666663</v>
       </c>
       <c r="E8" s="43">
-        <v>1.3</v>
-      </c>
-      <c r="F8" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="18">
+        <v>2</v>
+      </c>
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -5586,12 +5646,14 @@
       <c r="K8" s="18"/>
       <c r="L8" s="8">
         <f>100*SUM(E8:K8)/(2*A$1)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="M8" s="12">
-        <v>80</v>
-      </c>
-      <c r="N8" s="11"/>
+        <v>55</v>
+      </c>
+      <c r="N8" s="11">
+        <v>100</v>
+      </c>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="12"/>
@@ -5599,7 +5661,7 @@
       <c r="S8" s="11"/>
       <c r="T8" s="8">
         <f>SUM(M8:S8)/(A$1)</f>
-        <v>80</v>
+        <v>77.5</v>
       </c>
       <c r="U8" s="12"/>
       <c r="V8" s="11"/>
@@ -5622,30 +5684,32 @@
       <c r="AG8" s="12"/>
       <c r="AH8" s="17">
         <f>L8*0.1+T8*0.2+Z8*0.2+AF8*0.2+AG8*0.3</f>
-        <v>22.5</v>
+        <v>23</v>
       </c>
       <c r="AI8" s="17">
         <f>D8*0.4+AH8*0.6</f>
-        <v>37.659999999999997</v>
+        <v>41.826666666666668</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="D9" s="12">
-        <v>70.066666666666663</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="E9" s="43">
-        <v>1</v>
-      </c>
-      <c r="F9" s="18"/>
+        <v>1.3</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0</v>
+      </c>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
@@ -5653,12 +5717,14 @@
       <c r="K9" s="18"/>
       <c r="L9" s="8">
         <f>100*SUM(E9:K9)/(2*A$1)</f>
-        <v>50</v>
+        <v>32.5</v>
       </c>
       <c r="M9" s="12">
-        <v>55</v>
-      </c>
-      <c r="N9" s="11"/>
+        <v>80</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0</v>
+      </c>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
@@ -5666,7 +5732,7 @@
       <c r="S9" s="11"/>
       <c r="T9" s="8">
         <f>SUM(M9:S9)/(A$1)</f>
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="U9" s="12"/>
       <c r="V9" s="11"/>
@@ -5689,30 +5755,32 @@
       <c r="AG9" s="12"/>
       <c r="AH9" s="17">
         <f>L9*0.1+T9*0.2+Z9*0.2+AF9*0.2+AG9*0.3</f>
-        <v>16</v>
+        <v>11.25</v>
       </c>
       <c r="AI9" s="17">
         <f>D9*0.4+AH9*0.6</f>
-        <v>37.626666666666665</v>
+        <v>37.79</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="D10" s="12">
-        <v>87.283333333333331</v>
+        <v>70.55</v>
       </c>
       <c r="E10" s="43">
         <v>0</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="18">
+        <v>2</v>
+      </c>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
@@ -5720,12 +5788,14 @@
       <c r="K10" s="18"/>
       <c r="L10" s="8">
         <f>100*SUM(E10:K10)/(2*A$1)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M10" s="12">
         <v>0</v>
       </c>
-      <c r="N10" s="11"/>
+      <c r="N10" s="11">
+        <v>100</v>
+      </c>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
@@ -5733,7 +5803,7 @@
       <c r="S10" s="11"/>
       <c r="T10" s="8">
         <f>SUM(M10:S10)/(A$1)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="U10" s="12"/>
       <c r="V10" s="11"/>
@@ -5756,30 +5826,32 @@
       <c r="AG10" s="12"/>
       <c r="AH10" s="17">
         <f>L10*0.1+T10*0.2+Z10*0.2+AF10*0.2+AG10*0.3</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AI10" s="17">
         <f>D10*0.4+AH10*0.6</f>
-        <v>34.913333333333334</v>
+        <v>37.22</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="D11" s="12">
-        <v>84.833333333333343</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="E11" s="43">
-        <v>0</v>
-      </c>
-      <c r="F11" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="18">
+        <v>0</v>
+      </c>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
@@ -5787,12 +5859,14 @@
       <c r="K11" s="18"/>
       <c r="L11" s="8">
         <f>100*SUM(E11:K11)/(2*A$1)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M11" s="12">
-        <v>0</v>
-      </c>
-      <c r="N11" s="11"/>
+        <v>60</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0</v>
+      </c>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="12"/>
@@ -5800,7 +5874,7 @@
       <c r="S11" s="11"/>
       <c r="T11" s="8">
         <f>SUM(M11:S11)/(A$1)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U11" s="12"/>
       <c r="V11" s="11"/>
@@ -5823,30 +5897,32 @@
       <c r="AG11" s="12"/>
       <c r="AH11" s="17">
         <f>L11*0.1+T11*0.2+Z11*0.2+AF11*0.2+AG11*0.3</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="AI11" s="17">
         <f>D11*0.4+AH11*0.6</f>
-        <v>33.933333333333337</v>
+        <v>34.860000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>127</v>
+        <v>56</v>
       </c>
       <c r="D12" s="12">
-        <v>70.55</v>
+        <v>60.4</v>
       </c>
       <c r="E12" s="43">
-        <v>0</v>
-      </c>
-      <c r="F12" s="18"/>
+        <v>1.3</v>
+      </c>
+      <c r="F12" s="18">
+        <v>0</v>
+      </c>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
@@ -5854,12 +5930,14 @@
       <c r="K12" s="18"/>
       <c r="L12" s="8">
         <f>100*SUM(E12:K12)/(2*A$1)</f>
-        <v>0</v>
+        <v>32.5</v>
       </c>
       <c r="M12" s="12">
-        <v>0</v>
-      </c>
-      <c r="N12" s="11"/>
+        <v>80</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0</v>
+      </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
@@ -5867,7 +5945,7 @@
       <c r="S12" s="11"/>
       <c r="T12" s="8">
         <f>SUM(M12:S12)/(A$1)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="U12" s="12"/>
       <c r="V12" s="11"/>
@@ -5890,11 +5968,11 @@
       <c r="AG12" s="12"/>
       <c r="AH12" s="17">
         <f>L12*0.1+T12*0.2+Z12*0.2+AF12*0.2+AG12*0.3</f>
-        <v>0</v>
+        <v>11.25</v>
       </c>
       <c r="AI12" s="17">
         <f>D12*0.4+AH12*0.6</f>
-        <v>28.22</v>
+        <v>30.91</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5913,7 +5991,9 @@
       <c r="E13" s="43">
         <v>0</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="18">
+        <v>0</v>
+      </c>
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
@@ -5926,7 +6006,9 @@
       <c r="M13" s="12">
         <v>0</v>
       </c>
-      <c r="N13" s="11"/>
+      <c r="N13" s="11">
+        <v>0</v>
+      </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="12"/>
@@ -5980,7 +6062,9 @@
       <c r="E14" s="43">
         <v>0</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="F14" s="18">
+        <v>0</v>
+      </c>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
@@ -5993,7 +6077,9 @@
       <c r="M14" s="12">
         <v>0</v>
       </c>
-      <c r="N14" s="11"/>
+      <c r="N14" s="11">
+        <v>0</v>
+      </c>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="12"/>
@@ -6033,21 +6119,23 @@
     </row>
     <row r="15" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="D15" s="12">
-        <v>20.7</v>
+        <v>28.1</v>
       </c>
       <c r="E15" s="43">
-        <v>1</v>
-      </c>
-      <c r="F15" s="18"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="18">
+        <v>2</v>
+      </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
@@ -6058,9 +6146,11 @@
         <v>50</v>
       </c>
       <c r="M15" s="12">
-        <v>55</v>
-      </c>
-      <c r="N15" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="11">
+        <v>100</v>
+      </c>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="12"/>
@@ -6068,7 +6158,7 @@
       <c r="S15" s="11"/>
       <c r="T15" s="8">
         <f>SUM(M15:S15)/(A$1)</f>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="U15" s="12"/>
       <c r="V15" s="11"/>
@@ -6091,30 +6181,32 @@
       <c r="AG15" s="12"/>
       <c r="AH15" s="17">
         <f>L15*0.1+T15*0.2+Z15*0.2+AF15*0.2+AG15*0.3</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI15" s="17">
         <f>D15*0.4+AH15*0.6</f>
-        <v>17.88</v>
+        <v>20.240000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="D16" s="12">
-        <v>28.1</v>
+        <v>20.7</v>
       </c>
       <c r="E16" s="43">
-        <v>0</v>
-      </c>
-      <c r="F16" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="18">
+        <v>0</v>
+      </c>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
@@ -6122,12 +6214,14 @@
       <c r="K16" s="18"/>
       <c r="L16" s="8">
         <f>100*SUM(E16:K16)/(2*A$1)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M16" s="12">
-        <v>0</v>
-      </c>
-      <c r="N16" s="11"/>
+        <v>55</v>
+      </c>
+      <c r="N16" s="11">
+        <v>0</v>
+      </c>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="12"/>
@@ -6135,7 +6229,7 @@
       <c r="S16" s="11"/>
       <c r="T16" s="8">
         <f>SUM(M16:S16)/(A$1)</f>
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="U16" s="12"/>
       <c r="V16" s="11"/>
@@ -6158,11 +6252,11 @@
       <c r="AG16" s="12"/>
       <c r="AH16" s="17">
         <f>L16*0.1+T16*0.2+Z16*0.2+AF16*0.2+AG16*0.3</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI16" s="17">
         <f>D16*0.4+AH16*0.6</f>
-        <v>11.240000000000002</v>
+        <v>13.079999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:35" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6181,7 +6275,9 @@
       <c r="E17" s="43">
         <v>0</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="18">
+        <v>0</v>
+      </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -6194,7 +6290,9 @@
       <c r="M17" s="12">
         <v>0</v>
       </c>
-      <c r="N17" s="11"/>
+      <c r="N17" s="11">
+        <v>0</v>
+      </c>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="12"/>
@@ -6248,7 +6346,9 @@
       <c r="E18" s="43">
         <v>0</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="18">
+        <v>0</v>
+      </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
@@ -6261,7 +6361,9 @@
       <c r="M18" s="12">
         <v>0</v>
       </c>
-      <c r="N18" s="11"/>
+      <c r="N18" s="11">
+        <v>0</v>
+      </c>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
@@ -6315,7 +6417,9 @@
       <c r="E19" s="43">
         <v>0</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="18">
+        <v>0</v>
+      </c>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
@@ -6328,7 +6432,9 @@
       <c r="M19" s="12">
         <v>0</v>
       </c>
-      <c r="N19" s="12"/>
+      <c r="N19" s="11">
+        <v>0</v>
+      </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
@@ -6380,7 +6486,9 @@
       <c r="E20" s="43">
         <v>0</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="18">
+        <v>0</v>
+      </c>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -6393,7 +6501,9 @@
       <c r="M20" s="12">
         <v>0</v>
       </c>
-      <c r="N20" s="12"/>
+      <c r="N20" s="11">
+        <v>0</v>
+      </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
@@ -6447,7 +6557,9 @@
       <c r="E21" s="43">
         <v>0</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="18">
+        <v>0</v>
+      </c>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -6460,7 +6572,9 @@
       <c r="M21" s="12">
         <v>0</v>
       </c>
-      <c r="N21" s="12"/>
+      <c r="N21" s="11">
+        <v>0</v>
+      </c>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="12"/>
@@ -6514,7 +6628,9 @@
       <c r="E22" s="43">
         <v>0</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="18">
+        <v>0</v>
+      </c>
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
@@ -6527,7 +6643,9 @@
       <c r="M22" s="12">
         <v>0</v>
       </c>
-      <c r="N22" s="12"/>
+      <c r="N22" s="11">
+        <v>0</v>
+      </c>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="12"/>
@@ -6581,7 +6699,9 @@
       <c r="E23" s="43">
         <v>0</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="18">
+        <v>0</v>
+      </c>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
@@ -6594,7 +6714,9 @@
       <c r="M23" s="12">
         <v>0</v>
       </c>
-      <c r="N23" s="11"/>
+      <c r="N23" s="11">
+        <v>0</v>
+      </c>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="11"/>
@@ -6648,7 +6770,9 @@
       <c r="E24" s="43">
         <v>0</v>
       </c>
-      <c r="F24" s="18"/>
+      <c r="F24" s="18">
+        <v>0</v>
+      </c>
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
@@ -6661,7 +6785,9 @@
       <c r="M24" s="12">
         <v>0</v>
       </c>
-      <c r="N24" s="12"/>
+      <c r="N24" s="11">
+        <v>0</v>
+      </c>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
@@ -6715,7 +6841,9 @@
       <c r="E25" s="43">
         <v>0</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="F25" s="18">
+        <v>0</v>
+      </c>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
       <c r="I25" s="18"/>
@@ -6728,7 +6856,9 @@
       <c r="M25" s="12">
         <v>0</v>
       </c>
-      <c r="N25" s="12"/>
+      <c r="N25" s="11">
+        <v>0</v>
+      </c>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
@@ -6782,7 +6912,9 @@
       <c r="E26" s="43">
         <v>0</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="F26" s="18">
+        <v>0</v>
+      </c>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
@@ -6795,7 +6927,9 @@
       <c r="M26" s="12">
         <v>0</v>
       </c>
-      <c r="N26" s="12"/>
+      <c r="N26" s="11">
+        <v>0</v>
+      </c>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
@@ -6849,7 +6983,9 @@
       <c r="E27" s="43">
         <v>0</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="18">
+        <v>0</v>
+      </c>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
@@ -6862,7 +6998,9 @@
       <c r="M27" s="12">
         <v>0</v>
       </c>
-      <c r="N27" s="12"/>
+      <c r="N27" s="11">
+        <v>0</v>
+      </c>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="11"/>
@@ -6916,7 +7054,9 @@
       <c r="E28" s="43">
         <v>0</v>
       </c>
-      <c r="F28" s="18"/>
+      <c r="F28" s="18">
+        <v>0</v>
+      </c>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
@@ -6929,7 +7069,9 @@
       <c r="M28" s="12">
         <v>0</v>
       </c>
-      <c r="N28" s="12"/>
+      <c r="N28" s="11">
+        <v>0</v>
+      </c>
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="12"/>
@@ -6983,7 +7125,9 @@
       <c r="E29" s="43">
         <v>0</v>
       </c>
-      <c r="F29" s="18"/>
+      <c r="F29" s="18">
+        <v>0</v>
+      </c>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
@@ -6996,7 +7140,9 @@
       <c r="M29" s="12">
         <v>0</v>
       </c>
-      <c r="N29" s="12"/>
+      <c r="N29" s="11">
+        <v>0</v>
+      </c>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="12"/>
@@ -7050,7 +7196,9 @@
       <c r="E30" s="43">
         <v>0</v>
       </c>
-      <c r="F30" s="18"/>
+      <c r="F30" s="18">
+        <v>0</v>
+      </c>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
@@ -7063,7 +7211,9 @@
       <c r="M30" s="12">
         <v>0</v>
       </c>
-      <c r="N30" s="12"/>
+      <c r="N30" s="11">
+        <v>0</v>
+      </c>
       <c r="O30" s="12"/>
       <c r="P30" s="12"/>
       <c r="Q30" s="12"/>
@@ -7117,7 +7267,9 @@
       <c r="E31" s="43">
         <v>0</v>
       </c>
-      <c r="F31" s="18"/>
+      <c r="F31" s="18">
+        <v>0</v>
+      </c>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
@@ -7130,7 +7282,9 @@
       <c r="M31" s="12">
         <v>0</v>
       </c>
-      <c r="N31" s="12"/>
+      <c r="N31" s="11">
+        <v>0</v>
+      </c>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
@@ -7184,7 +7338,9 @@
       <c r="E32" s="43">
         <v>0</v>
       </c>
-      <c r="F32" s="18"/>
+      <c r="F32" s="18">
+        <v>0</v>
+      </c>
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
@@ -7197,7 +7353,9 @@
       <c r="M32" s="12">
         <v>0</v>
       </c>
-      <c r="N32" s="12"/>
+      <c r="N32" s="11">
+        <v>0</v>
+      </c>
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
       <c r="Q32" s="12"/>
@@ -7251,7 +7409,9 @@
       <c r="E33" s="43">
         <v>0</v>
       </c>
-      <c r="F33" s="18"/>
+      <c r="F33" s="18">
+        <v>0</v>
+      </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
       <c r="I33" s="18"/>
@@ -7264,7 +7424,9 @@
       <c r="M33" s="12">
         <v>0</v>
       </c>
-      <c r="N33" s="12"/>
+      <c r="N33" s="11">
+        <v>0</v>
+      </c>
       <c r="O33" s="12"/>
       <c r="P33" s="12"/>
       <c r="Q33" s="12"/>
@@ -7318,7 +7480,9 @@
       <c r="E34" s="43">
         <v>0</v>
       </c>
-      <c r="F34" s="18"/>
+      <c r="F34" s="18">
+        <v>0</v>
+      </c>
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
@@ -7331,7 +7495,9 @@
       <c r="M34" s="12">
         <v>0</v>
       </c>
-      <c r="N34" s="12"/>
+      <c r="N34" s="11">
+        <v>0</v>
+      </c>
       <c r="O34" s="12"/>
       <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
@@ -8706,14 +8872,14 @@
     <mergeCell ref="AA1:AF1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:K34">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8788,35 +8954,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:S34">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>80</formula>
       <formula>150</formula>
     </cfRule>

</xml_diff>